<commit_message>
arreglos pequeños proteus commit
</commit_message>
<xml_diff>
--- a/tabla_termocupla.xlsx
+++ b/tabla_termocupla.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andres D\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andres D\Documents\GitHub\ED3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4713EAF5-A98B-4751-BCD9-85C758026A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5263CC-C517-41A1-BC72-B3A4684C500D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2232" yWindow="2232" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,10 +114,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3830,8 +3830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4018,11 +4018,11 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
@@ -4043,10 +4043,10 @@
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>